<commit_message>
update pizza place sales sql code and dashboard
</commit_message>
<xml_diff>
--- a/Restaurant Sales Project/pizza place sales dashboard.xlsx
+++ b/Restaurant Sales Project/pizza place sales dashboard.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4c54a924b2259718/Documents/GitHub/proj-sql/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4c54a924b2259718/Documents/GitHub/proj-sql/Restaurant Sales Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="65" documentId="13_ncr:40009_{022BF68F-FDDD-45C2-A199-6F31013BF2E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{24FAE36C-0850-46C1-B0B5-EF75EED538E5}"/>
+  <xr:revisionPtr revIDLastSave="77" documentId="13_ncr:40009_{022BF68F-FDDD-45C2-A199-6F31013BF2E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CE505CB6-0AF7-41DE-9C89-0A3B9DEBC97F}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,10 +16,11 @@
     <sheet name="data_1" sheetId="1" state="hidden" r:id="rId1"/>
     <sheet name="data_2" sheetId="2" state="hidden" r:id="rId2"/>
     <sheet name="pizza_place_dashboard" sheetId="3" r:id="rId3"/>
-    <sheet name="data_3" sheetId="4" state="hidden" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId4"/>
+    <sheet name="data_3" sheetId="4" state="hidden" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">data_3!$A$1:$F$385</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">data_3!$A$1:$F$385</definedName>
     <definedName name="category">data_1!$A$2:$A$33</definedName>
     <definedName name="ingredients">data_1!$D$2:$D$33</definedName>
     <definedName name="month">data_3!$E$2:$E$385</definedName>
@@ -68,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1296" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1301" uniqueCount="146">
   <si>
     <t>category</t>
   </si>
@@ -491,6 +492,21 @@
   </si>
   <si>
     <t>Select a month:</t>
+  </si>
+  <si>
+    <t>One</t>
+  </si>
+  <si>
+    <t>Two</t>
+  </si>
+  <si>
+    <t>Three</t>
+  </si>
+  <si>
+    <t>Four</t>
+  </si>
+  <si>
+    <t>Five or more</t>
   </si>
 </sst>
 </file>
@@ -1436,20 +1452,6 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="t"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1878,20 +1880,6 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -2186,14 +2174,19 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Total revenue</a:t>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>Number of Pizzas per Order </a:t>
             </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> by pizza category</a:t>
+              <a:rPr lang="en-US" sz="1100" baseline="0"/>
+              <a:t> (Percentage) </a:t>
             </a:r>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -2229,201 +2222,80 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:pieChart>
-        <c:varyColors val="1"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:dPt>
-            <c:idx val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln w="12700">
               <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="75000"/>
-                  <a:alpha val="91000"/>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="50000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000001-ED85-4F6B-A47A-FBD46C5E8976}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="1"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="7030A0">
-                  <a:alpha val="77000"/>
-                </a:srgbClr>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000003-ED85-4F6B-A47A-FBD46C5E8976}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="2"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4">
-                  <a:lumMod val="75000"/>
-                  <a:alpha val="90000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000005-ED85-4F6B-A47A-FBD46C5E8976}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="3"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent6">
-                  <a:lumMod val="75000"/>
-                  <a:alpha val="93000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000007-ED85-4F6B-A47A-FBD46C5E8976}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="1"/>
-            <c:leaderLines>
-              <c:spPr>
-                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="35000"/>
-                      <a:lumOff val="65000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:round/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:leaderLines>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-            </c:extLst>
-          </c:dLbls>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>data_2!$E$29:$E$32</c:f>
+              <c:f>Sheet1!$A$1:$E$1</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Classic</c:v>
+                  <c:v>One</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Supreme</c:v>
+                  <c:v>Two</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Chicken</c:v>
+                  <c:v>Three</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Veggie</c:v>
+                  <c:v>Four</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Five or more</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data_2!$F$29:$F$32</c:f>
+              <c:f>Sheet1!$A$2:$E$2</c:f>
               <c:numCache>
-                <c:formatCode>_("$"* #,##0_);_("$"* \(#,##0\);_("$"* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>220053.1</c:v>
+                  <c:v>37.99</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>208197</c:v>
+                  <c:v>28.81</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>195919.5</c:v>
+                  <c:v>15.02</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>193690.45</c:v>
+                  <c:v>14.62</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.55</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000008-ED85-4F6B-A47A-FBD46C5E8976}"/>
+              <c16:uniqueId val="{00000008-7AB0-4B90-85EF-9F0379A3518B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2434,10 +2306,157 @@
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
-          <c:showLeaderLines val="1"/>
         </c:dLbls>
-        <c:firstSliceAng val="0"/>
-      </c:pieChart>
+        <c:gapWidth val="100"/>
+        <c:axId val="246651359"/>
+        <c:axId val="246669119"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="246651359"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="246669119"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="246669119"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>% of Total Orders</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="246651359"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -2446,37 +2465,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -2614,6 +2602,7 @@
             <a:solidFill>
               <a:schemeClr val="accent6">
                 <a:lumMod val="75000"/>
+                <a:alpha val="84000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:ln>
@@ -2761,8 +2750,145 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.4360269360269364E-2"/>
+                  <c:y val="-8.0983887430737825E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-4871-4DDB-8962-2E0D8D988614}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.436026936026944E-2"/>
+                  <c:y val="-6.2465368912219307E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-4871-4DDB-8962-2E0D8D988614}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="10"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.2255892255892408E-2"/>
+                  <c:y val="-9.487277631962672E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-4871-4DDB-8962-2E0D8D988614}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:numFmt formatCode="#,###" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>data_2!$E$36:$E$47</c:f>
@@ -2933,12 +3059,7 @@
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -2989,7 +3110,7 @@
         <c:numFmt formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
+        <c:tickLblPos val="none"/>
         <c:spPr>
           <a:noFill/>
           <a:ln>
@@ -5325,13 +5446,13 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>320040</xdr:colOff>
+      <xdr:colOff>601980</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>335280</xdr:colOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>15240</xdr:rowOff>
     </xdr:to>
@@ -5475,10 +5596,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6705,8 +6822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:V40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6810,7 +6927,7 @@
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="18" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
@@ -6825,12 +6942,12 @@
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B25" s="18" t="str" cm="1">
         <f t="array" ref="B25">_xlfn.XLOOKUP(D22&amp;LARGE(_xlfn._xlws.FILTER(sales,month=D22),1),month&amp;sales,pizzatype)</f>
-        <v>The Pepperoni Pizza</v>
+        <v>The Hawaiian Pizza</v>
       </c>
       <c r="C25" s="18"/>
       <c r="F25" s="18" cm="1">
         <f t="array" ref="F25">_xlfn.XLOOKUP(D22&amp;B25,month&amp;pizzatype,sales)</f>
-        <v>241</v>
+        <v>209</v>
       </c>
       <c r="G25" s="19"/>
     </row>
@@ -6849,7 +6966,7 @@
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B28" s="5" t="str">
         <f>VLOOKUP(B25,data_1!C2:D33,2,0)</f>
-        <v>Mozzarella Cheese, Pepperoni</v>
+        <v>Sliced Ham, Pineapple, Mozzarella Cheese</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
@@ -6966,6 +7083,58 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A42C4826-CD24-4784-A38E-1555C2C7A3B0}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>37.99</v>
+      </c>
+      <c r="B2">
+        <v>28.81</v>
+      </c>
+      <c r="C2">
+        <v>15.02</v>
+      </c>
+      <c r="D2">
+        <v>14.62</v>
+      </c>
+      <c r="E2">
+        <v>3.55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1AA1C2A-DE87-4517-B2ED-FAF2024B8244}">
   <dimension ref="A1:I385"/>
   <sheetViews>

</xml_diff>